<commit_message>
Added top scoring cotnext
</commit_message>
<xml_diff>
--- a/tex/tables/comparing space types (senti).xlsx
+++ b/tex/tables/comparing space types (senti).xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="num_stw_num_stw_50_D2VrepsDecis" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="sentiment" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">num_stw_num_stw_50_D2VrepsDecis!$A$1:$H$1</definedName>
@@ -4943,7 +4943,7 @@
   <dimension ref="A1:G507"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>